<commit_message>
Fix performance issue with file splitting. Delete prepare file feature (deprecated).
</commit_message>
<xml_diff>
--- a/report/stats_tmp.xlsx
+++ b/report/stats_tmp.xlsx
@@ -274,7 +274,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -328,11 +327,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103543936"/>
-        <c:axId val="103545856"/>
+        <c:axId val="105121664"/>
+        <c:axId val="105127936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103543936"/>
+        <c:axId val="105121664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,19 +357,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103545856"/>
+        <c:crossAx val="105127936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103545856"/>
+        <c:axId val="105127936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,14 +391,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103543936"/>
+        <c:crossAx val="105121664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -470,7 +467,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -512,11 +508,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106532224"/>
-        <c:axId val="106583168"/>
+        <c:axId val="105096704"/>
+        <c:axId val="105098240"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="106532224"/>
+        <c:axId val="105096704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +522,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106583168"/>
+        <c:crossAx val="105098240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -534,7 +530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106583168"/>
+        <c:axId val="105098240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,14 +553,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106532224"/>
+        <c:crossAx val="105096704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -616,7 +611,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -659,11 +653,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106615936"/>
-        <c:axId val="106617856"/>
+        <c:axId val="105114624"/>
+        <c:axId val="108287104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106615936"/>
+        <c:axId val="105114624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -689,19 +683,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106617856"/>
+        <c:crossAx val="108287104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106617856"/>
+        <c:axId val="108287104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,14 +717,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106615936"/>
+        <c:crossAx val="105114624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -763,7 +755,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -817,11 +808,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108018688"/>
-        <c:axId val="108020480"/>
+        <c:axId val="108316544"/>
+        <c:axId val="108322816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108018688"/>
+        <c:axId val="108316544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,19 +834,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108020480"/>
+        <c:crossAx val="108322816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108020480"/>
+        <c:axId val="108322816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,21 +868,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108018688"/>
+        <c:crossAx val="108316544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -960,6 +948,15 @@
             </c:strRef>
           </c:tx>
           <c:explosion val="25"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>AggregatedStatistics!$A$17:$A$23</c:f>
@@ -1004,7 +1001,7 @@
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
@@ -1058,7 +1055,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1108,11 +1104,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106192256"/>
-        <c:axId val="106218624"/>
+        <c:axId val="105168896"/>
+        <c:axId val="105170432"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="106192256"/>
+        <c:axId val="105168896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1118,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106218624"/>
+        <c:crossAx val="105170432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1130,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106218624"/>
+        <c:axId val="105170432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,14 +1149,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106192256"/>
+        <c:crossAx val="105168896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1192,7 +1187,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1246,11 +1240,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106378368"/>
-        <c:axId val="106380288"/>
+        <c:axId val="106509824"/>
+        <c:axId val="106511744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106378368"/>
+        <c:axId val="106509824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,19 +1266,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106380288"/>
+        <c:crossAx val="106511744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106380288"/>
+        <c:axId val="106511744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1307,21 +1300,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106378368"/>
+        <c:crossAx val="106509824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1371,7 +1362,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1421,11 +1411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103612416"/>
-        <c:axId val="103613952"/>
+        <c:axId val="106836352"/>
+        <c:axId val="106837888"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="103612416"/>
+        <c:axId val="106836352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1425,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103613952"/>
+        <c:crossAx val="106837888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1443,7 +1433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103613952"/>
+        <c:axId val="106837888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,14 +1456,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103612416"/>
+        <c:crossAx val="106836352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1546,7 +1535,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1600,11 +1588,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103627776"/>
-        <c:axId val="103650432"/>
+        <c:axId val="106846080"/>
+        <c:axId val="106868736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103627776"/>
+        <c:axId val="106846080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,19 +1614,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103650432"/>
+        <c:crossAx val="106868736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103650432"/>
+        <c:axId val="106868736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,14 +1648,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103627776"/>
+        <c:crossAx val="106846080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1700,7 +1686,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1754,11 +1739,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103659008"/>
-        <c:axId val="103660544"/>
+        <c:axId val="106889600"/>
+        <c:axId val="106891520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103659008"/>
+        <c:axId val="106889600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,19 +1765,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103660544"/>
+        <c:crossAx val="106891520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103660544"/>
+        <c:axId val="106891520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1815,21 +1799,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103659008"/>
+        <c:crossAx val="106889600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1879,7 +1861,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1933,11 +1914,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103736832"/>
-        <c:axId val="103738752"/>
+        <c:axId val="104877440"/>
+        <c:axId val="104879616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103736832"/>
+        <c:axId val="104877440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,19 +1940,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103738752"/>
+        <c:crossAx val="104879616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103738752"/>
+        <c:axId val="104879616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,14 +1974,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103736832"/>
+        <c:crossAx val="104877440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2101,7 +2080,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2151,11 +2129,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103780352"/>
-        <c:axId val="103781888"/>
+        <c:axId val="104891520"/>
+        <c:axId val="104893056"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="103780352"/>
+        <c:axId val="104891520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2165,7 +2143,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103781888"/>
+        <c:crossAx val="104893056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2173,7 +2151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103781888"/>
+        <c:axId val="104893056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,14 +2174,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103780352"/>
+        <c:crossAx val="104891520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2235,7 +2212,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2289,11 +2265,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106522112"/>
-        <c:axId val="106523648"/>
+        <c:axId val="105016704"/>
+        <c:axId val="105018880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106522112"/>
+        <c:axId val="105016704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,19 +2291,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106523648"/>
+        <c:crossAx val="105018880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106523648"/>
+        <c:axId val="105018880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,21 +2325,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106522112"/>
+        <c:crossAx val="105016704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2764,15 +2737,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3315,7 +3288,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>